<commit_message>
JR, ADD/INC/DEC bugs fixed
</commit_message>
<xml_diff>
--- a/opcodes.xlsx
+++ b/opcodes.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\themu\Documents\GitHub\RustBoy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61062E56-99B5-467F-B59A-23AC14A4AAEB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C6B4B16-3A91-499E-BDFC-DEC8AB53352D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2172" windowWidth="17280" windowHeight="8964" xr2:uid="{E2B97052-47AE-4DAE-845C-0659328573C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2B97052-47AE-4DAE-845C-0659328573C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="206">
   <si>
     <t>0x0</t>
   </si>
@@ -609,30 +610,6 @@
     <t>ADD A, u8</t>
   </si>
   <si>
-    <t>RST 00</t>
-  </si>
-  <si>
-    <t>RST 10</t>
-  </si>
-  <si>
-    <t>RST 20</t>
-  </si>
-  <si>
-    <t>RST 30</t>
-  </si>
-  <si>
-    <t>RST 18</t>
-  </si>
-  <si>
-    <t>RST 28</t>
-  </si>
-  <si>
-    <t>RST 38</t>
-  </si>
-  <si>
-    <t>RST 08</t>
-  </si>
-  <si>
     <t>Done(%):</t>
   </si>
   <si>
@@ -643,6 +620,36 @@
   </si>
   <si>
     <t>CB Prefix</t>
+  </si>
+  <si>
+    <t>RST 0x00</t>
+  </si>
+  <si>
+    <t>RST 0x10</t>
+  </si>
+  <si>
+    <t>RST 0x20</t>
+  </si>
+  <si>
+    <t>RST 0x30</t>
+  </si>
+  <si>
+    <t>RST 0x08</t>
+  </si>
+  <si>
+    <t>RST 0x18</t>
+  </si>
+  <si>
+    <t>RST 0x28</t>
+  </si>
+  <si>
+    <t>RST 0x38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -1156,12 +1163,14 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="17.33203125" style="3"/>
+    <col min="1" max="7" width="17.33203125" style="3"/>
+    <col min="8" max="8" width="17" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="17.33203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1788,7 +1797,7 @@
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="10" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="K14" s="10" t="s">
         <v>155</v>
@@ -1803,7 +1812,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1817,7 +1826,9 @@
       <c r="D15" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8" t="s">
+        <v>204</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="4" t="s">
         <v>100</v>
@@ -1825,18 +1836,22 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="10" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="M15" s="8"/>
+      <c r="M15" s="8" t="s">
+        <v>205</v>
+      </c>
       <c r="N15" s="1"/>
-      <c r="O15" s="8"/>
+      <c r="O15" s="8" t="s">
+        <v>205</v>
+      </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="10" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1852,8 +1867,12 @@
       <c r="D16" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="E16" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>205</v>
+      </c>
       <c r="G16" s="4" t="s">
         <v>101</v>
       </c>
@@ -1862,7 +1881,7 @@
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="10" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>143</v>
@@ -1870,14 +1889,20 @@
       <c r="L16" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
+      <c r="M16" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>205</v>
+      </c>
       <c r="P16" s="7" t="s">
         <v>129</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1894,7 +1919,9 @@
         <v>138</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>204</v>
+      </c>
       <c r="G17" s="4" t="s">
         <v>102</v>
       </c>
@@ -1903,7 +1930,7 @@
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="10" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>130</v>
@@ -1912,31 +1939,35 @@
         <v>141</v>
       </c>
       <c r="M17" s="1"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
+      <c r="N17" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>205</v>
+      </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="10" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="2" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E21" s="13">
         <f>((256 - COUNTBLANK(B2:Q17))/ 256)</f>
-        <v>0.71875</v>
+        <v>0.76171875</v>
       </c>
       <c r="F21" s="13">
         <f>((256 - COUNTBLANK(B25:Q40))/ 256)</f>

</xml_diff>